<commit_message>
new container, container search by barcode and small fixes.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_v3_4_1.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_v3_4_1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Container Creation Template</t>
   </si>
@@ -77,6 +77,9 @@
     <t xml:space="preserve">Freezer rack 2x4</t>
   </si>
   <si>
+    <t xml:space="preserve">Freezer rack 3x4</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freezer rack 4x4</t>
   </si>
   <si>
@@ -89,7 +92,13 @@
     <t xml:space="preserve">Freezer rack 7x4</t>
   </si>
   <si>
+    <t xml:space="preserve">Freezer rack 10x5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Freezer rack 8x6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freezer rack 11x6</t>
   </si>
   <si>
     <t xml:space="preserve">Freezer 3 shelves</t>
@@ -115,7 +124,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +199,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -296,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -358,6 +373,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,7 +463,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="22.33"/>
@@ -5076,7 +5095,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B107" type="list">
-      <formula1>Index!$A$2:$A$20</formula1>
+      <formula1>Index!$A$2:$A$23</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5095,13 +5114,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A1048576"/>
+  <dimension ref="A1:A1012"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>
@@ -5157,12 +5176,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>19</v>
       </c>
@@ -5172,7 +5191,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="s">
         <v>21</v>
       </c>
@@ -5182,34 +5201,46 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6187,7 +6218,9 @@
     <row r="1007" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1008" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1009" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
new container and sample kind
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Container_creation_v3_4_1.xlsx
+++ b/backend/fms_core/static/submission_templates/Container_creation_v3_4_1.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t xml:space="preserve">Container Creation Template</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tube box 10x10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tube box 21x10</t>
   </si>
   <si>
     <t xml:space="preserve">Tube rack 8x12</t>
@@ -124,7 +127,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -200,12 +203,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -221,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -269,6 +266,13 @@
       <right style="medium"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -344,7 +348,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,11 +360,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -373,10 +381,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -463,7 +467,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="22.33"/>
@@ -1514,11 +1518,11 @@
       <c r="A107" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="B107" s="8"/>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="12"/>
+      <c r="B107" s="11"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="4"/>
@@ -5095,7 +5099,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B8:B107" type="list">
-      <formula1>Index!$A$2:$A$23</formula1>
+      <formula1>Index!$A$2:$A$24</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -5114,55 +5118,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A1012"/>
+  <dimension ref="A1:A1013"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6484375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="9.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5171,77 +5175,81 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6221,6 +6229,7 @@
     <row r="1010" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1011" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1012" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>